<commit_message>
Added constants to Config file, pls read
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D68CDDB-A8A3-47C4-8E58-8DE32AD6B160}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDCC789-A923-4E60-8BEC-19F7B952730A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="1824" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>ProcessABCQueue</t>
@@ -128,13 +125,103 @@
   </si>
   <si>
     <t>URL for Epic Games store.</t>
+  </si>
+  <si>
+    <t>EpicChoice</t>
+  </si>
+  <si>
+    <t>SteamChoice</t>
+  </si>
+  <si>
+    <t>Epic Games</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Text that represents the text the user selects to choose the Epic launcher.</t>
+  </si>
+  <si>
+    <t>Text that represents the text the user selects to choose the Steam launcher.</t>
+  </si>
+  <si>
+    <t>Data/Temp/GamesToAdd.xlsx</t>
+  </si>
+  <si>
+    <t>A relative path for a workbook that stores free, unadded games fetched from multiple launchers in different sheets.</t>
+  </si>
+  <si>
+    <t>Data/Temp/FreeGames.xlsx</t>
+  </si>
+  <si>
+    <t>A relative path for a workbook that stores games marked to be added to a user's accounts.</t>
+  </si>
+  <si>
+    <t>WBAddOutputPath</t>
+  </si>
+  <si>
+    <t>WBInstallInputPath</t>
+  </si>
+  <si>
+    <t>WBInstallOutputPath</t>
+  </si>
+  <si>
+    <t>WBAddInputPath</t>
+  </si>
+  <si>
+    <t>WBGetOutputPath</t>
+  </si>
+  <si>
+    <t>WBEpicSheet</t>
+  </si>
+  <si>
+    <t>WBSteamSheet</t>
+  </si>
+  <si>
+    <t>A name to be used for sheets in each Workbook with Epic game lists.</t>
+  </si>
+  <si>
+    <t>A name to be used for sheets in each Workbook with Steam game lists.</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Data/Temp/GamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/GamesToInstall.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Output/GamesInstalled.xlsx</t>
+  </si>
+  <si>
+    <t>A relative path for a workbook that stores games successfully added to a user's accounts.</t>
+  </si>
+  <si>
+    <t>A relative path for a workbook that stores games marked to be installed to a user's accounts.</t>
+  </si>
+  <si>
+    <t>A relative path for a workbook that stores games successfully installed to a user's accounts.</t>
+  </si>
+  <si>
+    <t>SteamURL</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com</t>
+  </si>
+  <si>
+    <t>URL for Steam store.</t>
+  </si>
+  <si>
+    <t>GameGetter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -158,6 +245,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,10 +269,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -189,8 +283,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,16 +599,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
     <col min="3" max="3" width="81.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
@@ -553,13 +649,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -568,50 +664,130 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1577,10 +1753,17 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{9692FBA5-6394-4E04-B33E-EC247EB1FBE6}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{4B72A0D7-9D24-4992-881D-F70C0328B747}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1588,7 +1771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1640,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1664,7 +1849,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1686,7 +1871,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1697,7 +1882,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1708,14 +1893,34 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Moved SteamAddProject and nested workflows in main project
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDCC789-A923-4E60-8BEC-19F7B952730A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA7521E-3DB7-4DAB-87D9-E5D13AE446C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="1824" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="1824" windowWidth="17280" windowHeight="8976" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -215,6 +215,24 @@
   </si>
   <si>
     <t>GameGetter</t>
+  </si>
+  <si>
+    <t>Steam_Credential</t>
+  </si>
+  <si>
+    <t>Credentials to sign into steam</t>
+  </si>
+  <si>
+    <t>Steam_Failed_Credential</t>
+  </si>
+  <si>
+    <t>*FOR TESTING ONLY* Incorrect steam credentials to sign into steam</t>
+  </si>
+  <si>
+    <t>Steam_FilePath</t>
+  </si>
+  <si>
+    <t>File path to the steam application</t>
   </si>
 </sst>
 </file>
@@ -601,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C16" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -775,8 +793,28 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2903,7 +2941,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2947,7 +2987,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Modified Epic subprojs to implement library code, integrate into main process
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA7521E-3DB7-4DAB-87D9-E5D13AE446C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5C72B5-A40F-4C86-8B3F-B6A2DC3BD496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="1824" windowWidth="17280" windowHeight="8976" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>File path to the steam application</t>
+  </si>
+  <si>
+    <t>EpicCredential</t>
+  </si>
+  <si>
+    <t>Name for credential to sign into Epic Games</t>
+  </si>
+  <si>
+    <t>SteamCredential</t>
   </si>
 </sst>
 </file>
@@ -617,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C16" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -792,31 +801,48 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
       </c>
     </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1794,6 +1820,8 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -1809,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2941,7 +2969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Config file to add relevant constants
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5C72B5-A40F-4C86-8B3F-B6A2DC3BD496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237BFA82-FCEF-483D-A92E-34386DDBF017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -242,6 +242,18 @@
   </si>
   <si>
     <t>SteamCredential</t>
+  </si>
+  <si>
+    <t>StatusFailed</t>
+  </si>
+  <si>
+    <t>StatusSuccess</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Failure</t>
   </si>
 </sst>
 </file>
@@ -628,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1837,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1988,22 +2000,36 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Implemented Excel IO across all subprojects
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237BFA82-FCEF-483D-A92E-34386DDBF017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03127F36-0148-4476-833F-4F39F077CDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -145,33 +145,12 @@
     <t>Text that represents the text the user selects to choose the Steam launcher.</t>
   </si>
   <si>
-    <t>Data/Temp/GamesToAdd.xlsx</t>
-  </si>
-  <si>
     <t>A relative path for a workbook that stores free, unadded games fetched from multiple launchers in different sheets.</t>
   </si>
   <si>
-    <t>Data/Temp/FreeGames.xlsx</t>
-  </si>
-  <si>
     <t>A relative path for a workbook that stores games marked to be added to a user's accounts.</t>
   </si>
   <si>
-    <t>WBAddOutputPath</t>
-  </si>
-  <si>
-    <t>WBInstallInputPath</t>
-  </si>
-  <si>
-    <t>WBInstallOutputPath</t>
-  </si>
-  <si>
-    <t>WBAddInputPath</t>
-  </si>
-  <si>
-    <t>WBGetOutputPath</t>
-  </si>
-  <si>
     <t>WBEpicSheet</t>
   </si>
   <si>
@@ -184,18 +163,6 @@
     <t>A name to be used for sheets in each Workbook with Steam game lists.</t>
   </si>
   <si>
-    <t>Epic</t>
-  </si>
-  <si>
-    <t>Data/Temp/GamesAdded.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Temp/GamesToInstall.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Output/GamesInstalled.xlsx</t>
-  </si>
-  <si>
     <t>A relative path for a workbook that stores games successfully added to a user's accounts.</t>
   </si>
   <si>
@@ -254,6 +221,69 @@
   </si>
   <si>
     <t>Failure</t>
+  </si>
+  <si>
+    <t>EpicGetOutputPath</t>
+  </si>
+  <si>
+    <t>EpicAddInputPath</t>
+  </si>
+  <si>
+    <t>EpicAddOutputPath</t>
+  </si>
+  <si>
+    <t>EpicInstallInputPath</t>
+  </si>
+  <si>
+    <t>EpicInstallOutputPath</t>
+  </si>
+  <si>
+    <t>Data/Temp/Epic/FreeGames.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/Epic/GamesToAdd.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/Epic/GamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/Epic/GamesToInstall.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Output/Epic/GamesInstalled.xlsx</t>
+  </si>
+  <si>
+    <t>SteamGetOutputPath</t>
+  </si>
+  <si>
+    <t>SteamAddInputPath</t>
+  </si>
+  <si>
+    <t>SteamAddOutputPath</t>
+  </si>
+  <si>
+    <t>SteamInstallInputPath</t>
+  </si>
+  <si>
+    <t>SteamInstallOutputPath</t>
+  </si>
+  <si>
+    <t>Data/Temp/Steam/FreeGames.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/Steam/GamesToAdd.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/Steam/GamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/Steam/GamesToInstall.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Output/Steam/GamesInstalled.xlsx</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
@@ -638,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -703,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>23</v>
@@ -724,143 +754,193 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>71</v>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
       </c>
     </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1834,6 +1914,7 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -1849,7 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2002,18 +2083,18 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3043,13 +3124,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added list of statuses for workbook IO in Constants sheet
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03127F36-0148-4476-833F-4F39F077CDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9D2254-A079-4A5F-962C-93D07B22F7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Statuses</t>
+  </si>
+  <si>
+    <t>Retrieved, Added, Installed, Failed</t>
   </si>
 </sst>
 </file>
@@ -668,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -739,208 +745,210 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.4">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1914,12 +1922,11 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{9692FBA5-6394-4E04-B33E-EC247EB1FBE6}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{4B72A0D7-9D24-4992-881D-F70C0328B747}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{9692FBA5-6394-4E04-B33E-EC247EB1FBE6}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{4B72A0D7-9D24-4992-881D-F70C0328B747}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1930,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1981,7 +1988,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
@@ -2098,7 +2105,14 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
fixed subprojects to take in original Config instead of rereading the same file over and over
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9D2254-A079-4A5F-962C-93D07B22F7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24714B1B-71B1-49C4-B777-8456ABFCCB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,9 @@
     <t>A name to be used for sheets in each Workbook with Steam game lists.</t>
   </si>
   <si>
+    <t>Epic</t>
+  </si>
+  <si>
     <t>A relative path for a workbook that stores games successfully added to a user's accounts.</t>
   </si>
   <si>
@@ -286,10 +289,52 @@
     <t>Sheet1</t>
   </si>
   <si>
-    <t>Statuses</t>
-  </si>
-  <si>
-    <t>Retrieved, Added, Installed, Failed</t>
+    <t>StatusRetrieved</t>
+  </si>
+  <si>
+    <t>Retrieved</t>
+  </si>
+  <si>
+    <t>StatusAdded</t>
+  </si>
+  <si>
+    <t>StatusInstalled</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Installed</t>
+  </si>
+  <si>
+    <t>EpicGetOutputSheet</t>
+  </si>
+  <si>
+    <t>EpicAddInputSheet</t>
+  </si>
+  <si>
+    <t>EpicAddOutputSheet</t>
+  </si>
+  <si>
+    <t>EpicInstallInputSheet</t>
+  </si>
+  <si>
+    <t>EpicInstallOutputSheet</t>
+  </si>
+  <si>
+    <t>SteamGetOutputSheet</t>
+  </si>
+  <si>
+    <t>SteamAddInputSheet</t>
+  </si>
+  <si>
+    <t>SteamAddOutputSheet</t>
+  </si>
+  <si>
+    <t>SteamInstallInputSheet</t>
+  </si>
+  <si>
+    <t>SteamInstallOutputSheet</t>
   </si>
 </sst>
 </file>
@@ -674,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A6:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -722,97 +767,98 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="28.8">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.4">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.4">
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-    </row>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -826,148 +872,217 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" t="s">
         <v>45</v>
       </c>
     </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1922,11 +2037,19 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
+    <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{9692FBA5-6394-4E04-B33E-EC247EB1FBE6}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{4B72A0D7-9D24-4992-881D-F70C0328B747}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{9692FBA5-6394-4E04-B33E-EC247EB1FBE6}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{4B72A0D7-9D24-4992-881D-F70C0328B747}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1938,7 +2061,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2090,30 +2213,44 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3138,13 +3275,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated config file and argument values
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24714B1B-71B1-49C4-B777-8456ABFCCB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0182E6BF-4024-4CA2-BC2B-713EFF53DF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5535" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Data/Temp/Epic/GamesAdded.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/Epic/GamesToInstall.xlsx</t>
-  </si>
-  <si>
     <t>Data/Output/Epic/GamesInstalled.xlsx</t>
   </si>
   <si>
@@ -274,15 +271,9 @@
     <t>Data/Temp/Steam/FreeGames.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/Steam/GamesToAdd.xlsx</t>
-  </si>
-  <si>
     <t>Data/Temp/Steam/GamesAdded.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/Steam/GamesToInstall.xlsx</t>
-  </si>
-  <si>
     <t>Data/Output/Steam/GamesInstalled.xlsx</t>
   </si>
   <si>
@@ -335,6 +326,33 @@
   </si>
   <si>
     <t>SteamInstallOutputSheet</t>
+  </si>
+  <si>
+    <t>EpicGameList</t>
+  </si>
+  <si>
+    <t>Data/Input/EpicGameList.xlsx</t>
+  </si>
+  <si>
+    <t>SteamGameList</t>
+  </si>
+  <si>
+    <t>Data/Input/SteamGameList.xlsx</t>
+  </si>
+  <si>
+    <t>Relative path for list of free games on steam</t>
+  </si>
+  <si>
+    <t>Relative path for list of free games on Epic</t>
+  </si>
+  <si>
+    <t>Data/Temp/SteamGamesToAdd.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/EpicGamesToInstall.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/SteamGamesToInstall.xlsx</t>
   </si>
 </sst>
 </file>
@@ -719,18 +737,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1010"/>
+  <dimension ref="A1:Z1013"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -767,7 +785,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -778,7 +796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -817,7 +835,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -836,7 +854,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
@@ -855,7 +873,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
@@ -866,7 +884,7 @@
         <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
@@ -874,7 +892,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
@@ -885,7 +903,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
@@ -893,7 +911,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
@@ -902,10 +920,10 @@
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -913,7 +931,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -921,10 +939,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -932,7 +950,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -940,10 +958,10 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -951,7 +969,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -959,10 +977,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -970,7 +988,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
@@ -978,10 +996,10 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
@@ -989,7 +1007,7 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -998,86 +1016,106 @@
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-    </row>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
         <v>53</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>53</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
         <v>55</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>55</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C39" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2045,6 +2083,9 @@
     <row r="1008" ht="14.25" customHeight="1"/>
     <row r="1009" ht="14.25" customHeight="1"/>
     <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
+    <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="1013" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -2064,12 +2105,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2106,7 +2147,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2229,26 +2270,26 @@
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3231,12 +3272,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated file paths and argument values
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0182E6BF-4024-4CA2-BC2B-713EFF53DF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE7E13-AD04-4458-8C93-934A8AC3AA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5535" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,15 +244,6 @@
     <t>Data/Temp/Epic/FreeGames.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/Epic/GamesToAdd.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Temp/Epic/GamesAdded.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Output/Epic/GamesInstalled.xlsx</t>
-  </si>
-  <si>
     <t>SteamGetOutputPath</t>
   </si>
   <si>
@@ -271,12 +262,6 @@
     <t>Data/Temp/Steam/FreeGames.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/Steam/GamesAdded.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Output/Steam/GamesInstalled.xlsx</t>
-  </si>
-  <si>
     <t>Sheet1</t>
   </si>
   <si>
@@ -353,6 +338,21 @@
   </si>
   <si>
     <t>Data/Temp/SteamGamesToInstall.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Output/SteamGamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Output/SteamGamesInstalled.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Output/EpicGamesInstalled.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/EpicGamesToAdd.xlsx</t>
+  </si>
+  <si>
+    <t>Data/Temp/EpicGamesAdded.xlsx</t>
   </si>
 </sst>
 </file>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -835,7 +835,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -846,7 +846,7 @@
         <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
@@ -865,7 +865,7 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
@@ -884,7 +884,7 @@
         <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
@@ -903,7 +903,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
@@ -920,10 +920,10 @@
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -939,10 +939,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -958,10 +958,10 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -969,7 +969,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
@@ -996,10 +996,10 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -1016,24 +1016,24 @@
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
         <v>100</v>
-      </c>
-      <c r="B30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1042,7 +1042,7 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>43</v>
@@ -1053,7 +1053,7 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
@@ -2270,26 +2270,26 @@
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
set up test for table filter, to use between adding and installing games
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE7E13-AD04-4458-8C93-934A8AC3AA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD95AE3-B9E5-4507-AB64-38C40496C221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -151,18 +151,6 @@
     <t>A relative path for a workbook that stores games marked to be added to a user's accounts.</t>
   </si>
   <si>
-    <t>WBEpicSheet</t>
-  </si>
-  <si>
-    <t>WBSteamSheet</t>
-  </si>
-  <si>
-    <t>A name to be used for sheets in each Workbook with Epic game lists.</t>
-  </si>
-  <si>
-    <t>A name to be used for sheets in each Workbook with Steam game lists.</t>
-  </si>
-  <si>
     <t>Epic</t>
   </si>
   <si>
@@ -208,9 +196,6 @@
     <t>EpicCredential</t>
   </si>
   <si>
-    <t>Name for credential to sign into Epic Games</t>
-  </si>
-  <si>
     <t>SteamCredential</t>
   </si>
   <si>
@@ -262,9 +247,6 @@
     <t>Data/Temp/Steam/FreeGames.xlsx</t>
   </si>
   <si>
-    <t>Sheet1</t>
-  </si>
-  <si>
     <t>StatusRetrieved</t>
   </si>
   <si>
@@ -353,6 +335,9 @@
   </si>
   <si>
     <t>Data/Temp/EpicGamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Name for local credential to sign into Epic Games</t>
   </si>
 </sst>
 </file>
@@ -737,18 +722,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1013"/>
+  <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -785,18 +770,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -812,22 +797,22 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -835,18 +820,18 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -854,76 +839,76 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
         <v>72</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -931,7 +916,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -939,10 +924,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -950,7 +935,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -958,18 +943,18 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -977,18 +962,18 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
@@ -996,18 +981,18 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -1016,106 +1001,86 @@
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2083,9 +2048,6 @@
     <row r="1008" ht="14.25" customHeight="1"/>
     <row r="1009" ht="14.25" customHeight="1"/>
     <row r="1010" ht="14.25" customHeight="1"/>
-    <row r="1011" ht="14.25" customHeight="1"/>
-    <row r="1012" ht="14.25" customHeight="1"/>
-    <row r="1013" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -2105,12 +2067,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2147,7 +2109,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2254,42 +2216,42 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3272,12 +3234,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3316,13 +3278,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Trying to fix test
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE7E13-AD04-4458-8C93-934A8AC3AA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42025C68-136B-4B1E-B81D-5A1A661F98D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5535" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,21 +331,9 @@
     <t>Relative path for list of free games on Epic</t>
   </si>
   <si>
-    <t>Data/Temp/SteamGamesToAdd.xlsx</t>
-  </si>
-  <si>
     <t>Data/Temp/EpicGamesToInstall.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/SteamGamesToInstall.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Output/SteamGamesAdded.xlsx</t>
-  </si>
-  <si>
-    <t>Data/Output/SteamGamesInstalled.xlsx</t>
-  </si>
-  <si>
     <t>Data/Output/EpicGamesInstalled.xlsx</t>
   </si>
   <si>
@@ -353,6 +341,18 @@
   </si>
   <si>
     <t>Data/Temp/EpicGamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Temp\SteamGamesToAdd.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output\SteamGamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Temp\SteamGamesToInstall.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output\SteamGamesInstalled.xlsx</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
   <dimension ref="A1:Z1013"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -846,7 +846,7 @@
         <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -865,7 +865,7 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -884,7 +884,7 @@
         <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
@@ -903,7 +903,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
@@ -942,7 +942,7 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -961,7 +961,7 @@
         <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -980,7 +980,7 @@
         <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -999,7 +999,7 @@
         <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Fixed Excel IO when working with the user's input from the custom form
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66899B91-D1B0-46A6-9D69-F5E52E70D2FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAC4846-D270-4562-9457-F93166F3E9E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>A name to be used for sheets in each Workbook with Steam game lists.</t>
-  </si>
-  <si>
-    <t>Epic</t>
   </si>
   <si>
     <t>A relative path for a workbook that stores games successfully added to a user's accounts.</t>
@@ -745,16 +742,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -791,18 +788,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -818,22 +815,22 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" t="s">
         <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -841,18 +838,18 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -860,76 +857,76 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -937,18 +934,18 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -956,90 +953,90 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
         <v>97</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>98</v>
-      </c>
-      <c r="C29" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1048,7 +1045,7 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
         <v>43</v>
@@ -1059,7 +1056,7 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
@@ -1068,53 +1065,53 @@
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
         <v>53</v>
-      </c>
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
         <v>55</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" t="s">
         <v>109</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2118,12 +2115,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2160,7 +2157,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2267,42 +2264,42 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
         <v>63</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3285,12 +3282,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3329,13 +3326,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Removed QueueItems from main process, replaced with sample DataRow with one column
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B5182C-6DD9-4248-8747-D04A683979A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C26B939-F73D-4A4B-8C79-AB802E49A969}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="3480" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -742,16 +742,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -788,7 +788,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -799,7 +799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2111,16 +2111,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2157,12 +2157,12 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
@@ -3282,12 +3282,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Fixed multipe write issue
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C26B939-F73D-4A4B-8C79-AB802E49A969}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D42FA34-1D08-4F00-B8F1-F3187BA8DDE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -151,18 +151,6 @@
     <t>A relative path for a workbook that stores games marked to be added to a user's accounts.</t>
   </si>
   <si>
-    <t>WBEpicSheet</t>
-  </si>
-  <si>
-    <t>WBSteamSheet</t>
-  </si>
-  <si>
-    <t>A name to be used for sheets in each Workbook with Epic game lists.</t>
-  </si>
-  <si>
-    <t>A name to be used for sheets in each Workbook with Steam game lists.</t>
-  </si>
-  <si>
     <t>A relative path for a workbook that stores games successfully added to a user's accounts.</t>
   </si>
   <si>
@@ -310,24 +298,6 @@
     <t>SteamInstallOutputSheet</t>
   </si>
   <si>
-    <t>EpicGameList</t>
-  </si>
-  <si>
-    <t>Data/Input/EpicGameList.xlsx</t>
-  </si>
-  <si>
-    <t>SteamGameList</t>
-  </si>
-  <si>
-    <t>Data/Input/SteamGameList.xlsx</t>
-  </si>
-  <si>
-    <t>Relative path for list of free games on steam</t>
-  </si>
-  <si>
-    <t>Relative path for list of free games on Epic</t>
-  </si>
-  <si>
     <t>Data/Temp/EpicGamesToInstall.xlsx</t>
   </si>
   <si>
@@ -337,9 +307,6 @@
     <t>Data/Temp/EpicGamesToAdd.xlsx</t>
   </si>
   <si>
-    <t>Data/Temp/EpicGamesAdded.xlsx</t>
-  </si>
-  <si>
     <t>Data\Temp\SteamGamesToAdd.xlsx</t>
   </si>
   <si>
@@ -356,6 +323,9 @@
   </si>
   <si>
     <t>C:\Program Files (x86)\Steam\steam.exe</t>
+  </si>
+  <si>
+    <t>Data/Output/EpicGamesAdded.xlsx</t>
   </si>
 </sst>
 </file>
@@ -740,18 +710,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1013"/>
+  <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -788,18 +758,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -815,22 +785,22 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -838,262 +808,195 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-    </row>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>77</v>
-      </c>
-    </row>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-    </row>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
         <v>72</v>
       </c>
-      <c r="B20" t="s">
-        <v>104</v>
-      </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" t="s">
-        <v>53</v>
-      </c>
-    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
         <v>54</v>
@@ -1108,28 +1011,55 @@
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
@@ -2096,6 +2026,10 @@
     <row r="1011" ht="14.25" customHeight="1"/>
     <row r="1012" ht="14.25" customHeight="1"/>
     <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
+    <row r="1016" ht="14.25" customHeight="1"/>
+    <row r="1017" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -2111,16 +2045,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2157,7 +2091,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2264,42 +2198,42 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3282,12 +3216,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3326,13 +3260,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
fixed ReportToUser to not hardcode credential and ask user for email
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D42FA34-1D08-4F00-B8F1-F3187BA8DDE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85299D43-0E93-42A9-9CF3-03D020C4C896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -326,6 +326,15 @@
   </si>
   <si>
     <t>Data/Output/EpicGamesAdded.xlsx</t>
+  </si>
+  <si>
+    <t>EmailCredential</t>
+  </si>
+  <si>
+    <t>GGEmailCredential</t>
+  </si>
+  <si>
+    <t>Name of the credential asset used to send emails to the user.</t>
   </si>
 </sst>
 </file>
@@ -712,16 +721,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -758,7 +767,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -769,7 +778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -992,7 +1001,17 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2049,12 +2068,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2091,7 +2110,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3216,12 +3235,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
attempt to run main process from orchestrator as a job
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85299D43-0E93-42A9-9CF3-03D020C4C896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF0F9B3-1792-42B1-8D43-B8E7CDCB4CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -721,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -2064,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2115,7 +2115,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Removed unused asset from Config
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF0F9B3-1792-42B1-8D43-B8E7CDCB4CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB04C2D-BED6-407E-A1C3-42C9377A0944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26490" yWindow="3150" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -182,12 +182,6 @@
   </si>
   <si>
     <t>*FOR TESTING ONLY* Incorrect steam credentials to sign into steam</t>
-  </si>
-  <si>
-    <t>Steam_FilePath</t>
-  </si>
-  <si>
-    <t>File path to the steam application</t>
   </si>
   <si>
     <t>EpicCredential</t>
@@ -806,10 +800,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -817,19 +811,19 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
@@ -837,18 +831,18 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -856,19 +850,19 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
@@ -876,18 +870,18 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
@@ -895,19 +889,19 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -915,19 +909,19 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
@@ -935,18 +929,18 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -954,19 +948,19 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
         <v>42</v>
@@ -974,18 +968,18 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
         <v>43</v>
@@ -993,23 +987,23 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
         <v>100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1018,22 +1012,22 @@
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
@@ -1061,10 +1055,10 @@
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2064,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2217,42 +2211,42 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
         <v>76</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
         <v>77</v>
-      </c>
-      <c r="B21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3231,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3277,17 +3271,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Changed log message when primary process starts for clarity of logical flow
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Config.xlsx
+++ b/GameGetter/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB04C2D-BED6-407E-A1C3-42C9377A0944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25293823-D3C9-40E4-84E2-9332726C4A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26490" yWindow="3150" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26490" yWindow="3150" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>Name of the credential asset used to send emails to the user.</t>
+  </si>
+  <si>
+    <t>LogMessage_BeginMainProcess</t>
+  </si>
+  <si>
+    <t>Beginning GameGetter primary process…</t>
   </si>
 </sst>
 </file>
@@ -2058,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2183,7 +2189,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -3225,7 +3238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>